<commit_message>
added jobless job seeker map
</commit_message>
<xml_diff>
--- a/03 - Interactive Viz/2_1 Taux de chomage_all.xlsx
+++ b/03 - Interactive Viz/2_1 Taux de chomage_all.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="62">
   <si>
     <t>2.1 Taux de chômage</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t xml:space="preserve">Demandeurs d'emploi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demandeurs d'emploi non chômeurs - gain intermédiaire</t>
   </si>
   <si>
     <t xml:space="preserve">Zurich</t>
@@ -242,7 +245,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -273,7 +276,7 @@
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H3" t="s">
         <v>4</v>
@@ -282,6 +285,12 @@
         <v>4</v>
       </c>
       <c r="J3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -303,28 +312,34 @@
         <v>9</v>
       </c>
       <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
         <v>6</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>7</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>8</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>9</v>
+      </c>
+      <c r="L4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5"/>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1">
         <v>27225</v>
@@ -332,29 +347,35 @@
       <c r="F5" s="1">
         <v>34156</v>
       </c>
-      <c r="G5" t="s">
-        <v>11</v>
+      <c r="G5" s="1">
+        <v>3984</v>
       </c>
       <c r="H5" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="1">
         <v>27225</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>34156</v>
+      </c>
+      <c r="L5" s="1">
+        <v>3984</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6"/>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E6" s="1">
         <v>13658</v>
@@ -362,29 +383,35 @@
       <c r="F6" s="1">
         <v>18385</v>
       </c>
-      <c r="G6" t="s">
-        <v>14</v>
+      <c r="G6" s="1">
+        <v>2142</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="1">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="1">
         <v>13658</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <v>18385</v>
+      </c>
+      <c r="L6" s="1">
+        <v>2142</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7"/>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="1">
         <v>3885</v>
@@ -392,29 +419,35 @@
       <c r="F7" s="1">
         <v>6756</v>
       </c>
-      <c r="G7" t="s">
-        <v>16</v>
+      <c r="G7" s="1">
+        <v>1134</v>
       </c>
       <c r="H7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="1">
+        <v>17</v>
+      </c>
+      <c r="I7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="1">
         <v>3885</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <v>6756</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1134</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8"/>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8" s="1">
         <v>112</v>
@@ -422,29 +455,35 @@
       <c r="F8" s="1">
         <v>257</v>
       </c>
-      <c r="G8" t="s">
-        <v>18</v>
+      <c r="G8" s="1">
+        <v>67</v>
       </c>
       <c r="H8" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="1">
         <v>112</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K8" s="1">
         <v>257</v>
+      </c>
+      <c r="L8" s="1">
+        <v>67</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9"/>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E9" s="1">
         <v>1455</v>
@@ -452,29 +491,35 @@
       <c r="F9" s="1">
         <v>2229</v>
       </c>
-      <c r="G9" t="s">
-        <v>16</v>
+      <c r="G9" s="1">
+        <v>264</v>
       </c>
       <c r="H9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="1">
+        <v>17</v>
+      </c>
+      <c r="I9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="1">
         <v>1455</v>
       </c>
-      <c r="J9" s="1">
+      <c r="K9" s="1">
         <v>2229</v>
+      </c>
+      <c r="L9" s="1">
+        <v>264</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10"/>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E10" s="1">
         <v>153</v>
@@ -482,29 +527,35 @@
       <c r="F10" s="1">
         <v>319</v>
       </c>
-      <c r="G10" t="s">
-        <v>22</v>
+      <c r="G10" s="1">
+        <v>26</v>
       </c>
       <c r="H10" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="1">
         <v>153</v>
       </c>
-      <c r="J10" s="1">
+      <c r="K10" s="1">
         <v>319</v>
+      </c>
+      <c r="L10" s="1">
+        <v>26</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11"/>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1">
         <v>248</v>
@@ -512,29 +563,35 @@
       <c r="F11" s="1">
         <v>436</v>
       </c>
-      <c r="G11" t="s">
-        <v>25</v>
+      <c r="G11" s="1">
+        <v>28</v>
       </c>
       <c r="H11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11" s="1">
+        <v>26</v>
+      </c>
+      <c r="I11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="1">
         <v>248</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
         <v>436</v>
+      </c>
+      <c r="L11" s="1">
+        <v>28</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12"/>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E12" s="1">
         <v>416</v>
@@ -542,29 +599,35 @@
       <c r="F12" s="1">
         <v>713</v>
       </c>
-      <c r="G12" t="s">
-        <v>27</v>
+      <c r="G12" s="1">
+        <v>154</v>
       </c>
       <c r="H12" t="s">
-        <v>23</v>
-      </c>
-      <c r="I12" s="1">
+        <v>28</v>
+      </c>
+      <c r="I12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="1">
         <v>416</v>
       </c>
-      <c r="J12" s="1">
+      <c r="K12" s="1">
         <v>713</v>
+      </c>
+      <c r="L12" s="1">
+        <v>154</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13"/>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E13" s="1">
         <v>1543</v>
@@ -572,29 +635,35 @@
       <c r="F13" s="1">
         <v>2615</v>
       </c>
-      <c r="G13" t="s">
-        <v>29</v>
+      <c r="G13" s="1">
+        <v>391</v>
       </c>
       <c r="H13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" s="1">
+        <v>30</v>
+      </c>
+      <c r="I13" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="1">
         <v>1543</v>
       </c>
-      <c r="J13" s="1">
+      <c r="K13" s="1">
         <v>2615</v>
+      </c>
+      <c r="L13" s="1">
+        <v>391</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14"/>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E14" s="1">
         <v>4466</v>
@@ -602,29 +671,35 @@
       <c r="F14" s="1">
         <v>7837</v>
       </c>
-      <c r="G14" t="s">
-        <v>31</v>
+      <c r="G14" s="1">
+        <v>1798</v>
       </c>
       <c r="H14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" s="1">
+        <v>32</v>
+      </c>
+      <c r="I14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="1">
         <v>4466</v>
       </c>
-      <c r="J14" s="1">
+      <c r="K14" s="1">
         <v>7837</v>
+      </c>
+      <c r="L14" s="1">
+        <v>1798</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B15"/>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E15" s="1">
         <v>3801</v>
@@ -632,29 +707,35 @@
       <c r="F15" s="1">
         <v>6628</v>
       </c>
-      <c r="G15" t="s">
-        <v>33</v>
+      <c r="G15" s="1">
+        <v>1637</v>
       </c>
       <c r="H15" t="s">
-        <v>12</v>
-      </c>
-      <c r="I15" s="1">
+        <v>34</v>
+      </c>
+      <c r="I15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" s="1">
         <v>3801</v>
       </c>
-      <c r="J15" s="1">
+      <c r="K15" s="1">
         <v>6628</v>
+      </c>
+      <c r="L15" s="1">
+        <v>1637</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B16"/>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E16" s="1">
         <v>3455</v>
@@ -662,29 +743,35 @@
       <c r="F16" s="1">
         <v>5168</v>
       </c>
-      <c r="G16" t="s">
-        <v>35</v>
+      <c r="G16" s="1">
+        <v>1136</v>
       </c>
       <c r="H16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I16" s="1">
+        <v>36</v>
+      </c>
+      <c r="I16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="1">
         <v>3455</v>
       </c>
-      <c r="J16" s="1">
+      <c r="K16" s="1">
         <v>5168</v>
+      </c>
+      <c r="L16" s="1">
+        <v>1136</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B17"/>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E17" s="1">
         <v>4082</v>
@@ -692,29 +779,35 @@
       <c r="F17" s="1">
         <v>5540</v>
       </c>
-      <c r="G17" t="s">
-        <v>37</v>
+      <c r="G17" s="1">
+        <v>1088</v>
       </c>
       <c r="H17" t="s">
-        <v>12</v>
-      </c>
-      <c r="I17" s="1">
+        <v>38</v>
+      </c>
+      <c r="I17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" s="1">
         <v>4082</v>
       </c>
-      <c r="J17" s="1">
+      <c r="K17" s="1">
         <v>5540</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1088</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B18"/>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E18" s="1">
         <v>1286</v>
@@ -722,29 +815,35 @@
       <c r="F18" s="1">
         <v>2328</v>
       </c>
-      <c r="G18" t="s">
-        <v>39</v>
+      <c r="G18" s="1">
+        <v>488</v>
       </c>
       <c r="H18" t="s">
-        <v>23</v>
-      </c>
-      <c r="I18" s="1">
+        <v>40</v>
+      </c>
+      <c r="I18" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="1">
         <v>1286</v>
       </c>
-      <c r="J18" s="1">
+      <c r="K18" s="1">
         <v>2328</v>
+      </c>
+      <c r="L18" s="1">
+        <v>488</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B19"/>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E19" s="1">
         <v>523</v>
@@ -752,29 +851,35 @@
       <c r="F19" s="1">
         <v>866</v>
       </c>
-      <c r="G19" t="s">
-        <v>16</v>
+      <c r="G19" s="1">
+        <v>155</v>
       </c>
       <c r="H19" t="s">
-        <v>23</v>
-      </c>
-      <c r="I19" s="1">
+        <v>17</v>
+      </c>
+      <c r="I19" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" s="1">
         <v>523</v>
       </c>
-      <c r="J19" s="1">
+      <c r="K19" s="1">
         <v>866</v>
+      </c>
+      <c r="L19" s="1">
+        <v>155</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B20"/>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E20" s="1">
         <v>62</v>
@@ -782,29 +887,35 @@
       <c r="F20" s="1">
         <v>102</v>
       </c>
-      <c r="G20" t="s">
-        <v>22</v>
+      <c r="G20" s="1">
+        <v>36</v>
       </c>
       <c r="H20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I20" s="1">
+        <v>23</v>
+      </c>
+      <c r="I20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="1">
         <v>62</v>
       </c>
-      <c r="J20" s="1">
+      <c r="K20" s="1">
         <v>102</v>
+      </c>
+      <c r="L20" s="1">
+        <v>36</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B21"/>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E21" s="1">
         <v>6127</v>
@@ -812,29 +923,35 @@
       <c r="F21" s="1">
         <v>10363</v>
       </c>
-      <c r="G21" t="s">
-        <v>43</v>
+      <c r="G21" s="1">
+        <v>1857</v>
       </c>
       <c r="H21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I21" s="1">
+        <v>44</v>
+      </c>
+      <c r="I21" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" s="1">
         <v>6127</v>
       </c>
-      <c r="J21" s="1">
+      <c r="K21" s="1">
         <v>10363</v>
+      </c>
+      <c r="L21" s="1">
+        <v>1857</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B22"/>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E22" s="1">
         <v>1166</v>
@@ -842,29 +959,35 @@
       <c r="F22" s="1">
         <v>2590</v>
       </c>
-      <c r="G22" t="s">
-        <v>45</v>
+      <c r="G22" s="1">
+        <v>776</v>
       </c>
       <c r="H22" t="s">
-        <v>12</v>
-      </c>
-      <c r="I22" s="1">
+        <v>46</v>
+      </c>
+      <c r="I22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J22" s="1">
         <v>1166</v>
       </c>
-      <c r="J22" s="1">
+      <c r="K22" s="1">
         <v>2590</v>
+      </c>
+      <c r="L22" s="1">
+        <v>776</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B23"/>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E23" s="1">
         <v>10684</v>
@@ -872,29 +995,35 @@
       <c r="F23" s="1">
         <v>15145</v>
       </c>
-      <c r="G23" t="s">
-        <v>47</v>
+      <c r="G23" s="1">
+        <v>2678</v>
       </c>
       <c r="H23" t="s">
-        <v>12</v>
-      </c>
-      <c r="I23" s="1">
+        <v>48</v>
+      </c>
+      <c r="I23" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" s="1">
         <v>10684</v>
       </c>
-      <c r="J23" s="1">
+      <c r="K23" s="1">
         <v>15145</v>
+      </c>
+      <c r="L23" s="1">
+        <v>2678</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B24"/>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E24" s="1">
         <v>3058</v>
@@ -902,29 +1031,35 @@
       <c r="F24" s="1">
         <v>5618</v>
       </c>
-      <c r="G24" t="s">
-        <v>49</v>
+      <c r="G24" s="1">
+        <v>1365</v>
       </c>
       <c r="H24" t="s">
-        <v>12</v>
-      </c>
-      <c r="I24" s="1">
+        <v>50</v>
+      </c>
+      <c r="I24" t="s">
+        <v>13</v>
+      </c>
+      <c r="J24" s="1">
         <v>3058</v>
       </c>
-      <c r="J24" s="1">
+      <c r="K24" s="1">
         <v>5618</v>
+      </c>
+      <c r="L24" s="1">
+        <v>1365</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B25"/>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E25" s="1">
         <v>5202</v>
@@ -932,29 +1067,35 @@
       <c r="F25" s="1">
         <v>8675</v>
       </c>
-      <c r="G25" t="s">
-        <v>51</v>
+      <c r="G25" s="1">
+        <v>1896</v>
       </c>
       <c r="H25" t="s">
-        <v>12</v>
-      </c>
-      <c r="I25" s="1">
+        <v>52</v>
+      </c>
+      <c r="I25" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25" s="1">
         <v>5202</v>
       </c>
-      <c r="J25" s="1">
+      <c r="K25" s="1">
         <v>8675</v>
+      </c>
+      <c r="L25" s="1">
+        <v>1896</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B26"/>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E26" s="1">
         <v>17155</v>
@@ -962,29 +1103,35 @@
       <c r="F26" s="1">
         <v>24649</v>
       </c>
-      <c r="G26" t="s">
-        <v>53</v>
+      <c r="G26" s="1">
+        <v>4959</v>
       </c>
       <c r="H26" t="s">
-        <v>12</v>
-      </c>
-      <c r="I26" s="1">
+        <v>54</v>
+      </c>
+      <c r="I26" t="s">
+        <v>13</v>
+      </c>
+      <c r="J26" s="1">
         <v>17155</v>
       </c>
-      <c r="J26" s="1">
+      <c r="K26" s="1">
         <v>24649</v>
+      </c>
+      <c r="L26" s="1">
+        <v>4959</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B27"/>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E27" s="1">
         <v>4816</v>
@@ -992,29 +1139,35 @@
       <c r="F27" s="1">
         <v>8027</v>
       </c>
-      <c r="G27" t="s">
-        <v>37</v>
+      <c r="G27" s="1">
+        <v>1954</v>
       </c>
       <c r="H27" t="s">
-        <v>12</v>
-      </c>
-      <c r="I27" s="1">
+        <v>38</v>
+      </c>
+      <c r="I27" t="s">
+        <v>13</v>
+      </c>
+      <c r="J27" s="1">
         <v>4816</v>
       </c>
-      <c r="J27" s="1">
+      <c r="K27" s="1">
         <v>8027</v>
+      </c>
+      <c r="L27" s="1">
+        <v>1954</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B28"/>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E28" s="1">
         <v>4738</v>
@@ -1022,29 +1175,35 @@
       <c r="F28" s="1">
         <v>6350</v>
       </c>
-      <c r="G28" t="s">
-        <v>56</v>
+      <c r="G28" s="1">
+        <v>1030</v>
       </c>
       <c r="H28" t="s">
-        <v>12</v>
-      </c>
-      <c r="I28" s="1">
+        <v>57</v>
+      </c>
+      <c r="I28" t="s">
+        <v>13</v>
+      </c>
+      <c r="J28" s="1">
         <v>4738</v>
       </c>
-      <c r="J28" s="1">
+      <c r="K28" s="1">
         <v>6350</v>
+      </c>
+      <c r="L28" s="1">
+        <v>1030</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B29"/>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E29" s="1">
         <v>12234</v>
@@ -1052,29 +1211,35 @@
       <c r="F29" s="1">
         <v>15497</v>
       </c>
-      <c r="G29" t="s">
-        <v>58</v>
+      <c r="G29" s="1">
+        <v>2023</v>
       </c>
       <c r="H29" t="s">
-        <v>12</v>
-      </c>
-      <c r="I29" s="1">
+        <v>59</v>
+      </c>
+      <c r="I29" t="s">
+        <v>13</v>
+      </c>
+      <c r="J29" s="1">
         <v>12234</v>
       </c>
-      <c r="J29" s="1">
+      <c r="K29" s="1">
         <v>15497</v>
+      </c>
+      <c r="L29" s="1">
+        <v>2023</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B30"/>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D30" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E30" s="1">
         <v>1619</v>
@@ -1082,17 +1247,23 @@
       <c r="F30" s="1">
         <v>2375</v>
       </c>
-      <c r="G30" t="s">
-        <v>60</v>
+      <c r="G30" s="1">
+        <v>351</v>
       </c>
       <c r="H30" t="s">
-        <v>23</v>
-      </c>
-      <c r="I30" s="1">
+        <v>61</v>
+      </c>
+      <c r="I30" t="s">
+        <v>24</v>
+      </c>
+      <c r="J30" s="1">
         <v>1619</v>
       </c>
-      <c r="J30" s="1">
+      <c r="K30" s="1">
         <v>2375</v>
+      </c>
+      <c r="L30" s="1">
+        <v>351</v>
       </c>
     </row>
     <row r="31">
@@ -1101,10 +1272,10 @@
       </c>
       <c r="B31"/>
       <c r="C31" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E31" s="1">
         <v>133169</v>
@@ -1112,17 +1283,23 @@
       <c r="F31" s="1">
         <v>193624</v>
       </c>
-      <c r="G31" t="s">
-        <v>39</v>
+      <c r="G31" s="1">
+        <v>33417</v>
       </c>
       <c r="H31" t="s">
-        <v>12</v>
-      </c>
-      <c r="I31" s="1">
+        <v>40</v>
+      </c>
+      <c r="I31" t="s">
+        <v>13</v>
+      </c>
+      <c r="J31" s="1">
         <v>133169</v>
       </c>
-      <c r="J31" s="1">
+      <c r="K31" s="1">
         <v>193624</v>
+      </c>
+      <c r="L31" s="1">
+        <v>33417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>